<commit_message>
Update Tabel Pemesanan Tiket Kereta.xlsx
</commit_message>
<xml_diff>
--- a/Tabel Pemesanan Tiket Kereta.xlsx
+++ b/Tabel Pemesanan Tiket Kereta.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tugas dan Materi\Semester 5\Sistem Basis Data\UTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tugas dan Materi\UPI 2016\Semester 5\Sistem Basis Data\UTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0245ACD-7644-4544-96ED-20AC68CA1481}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239F00BD-C156-475E-9457-7B359F64980F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="4992" xr2:uid="{C41C43FE-8CAB-4197-8FAD-5B8E71EE3CBE}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="78">
   <si>
     <t>Customer</t>
   </si>
@@ -159,9 +159,6 @@
     <t>id_pemesanan</t>
   </si>
   <si>
-    <t>Integer(1)  Not Null Unsigned</t>
-  </si>
-  <si>
     <t>Char(20) Not Null</t>
   </si>
   <si>
@@ -361,6 +358,21 @@
   </si>
   <si>
     <t>Jadwal</t>
+  </si>
+  <si>
+    <t>id_kereta</t>
+  </si>
+  <si>
+    <t>Enum('Tersedia' , 'Penuh') Default 'Tersedia'</t>
+  </si>
+  <si>
+    <t>id_jadwal</t>
+  </si>
+  <si>
+    <t>harga_tiket</t>
+  </si>
+  <si>
+    <t>id_harga</t>
   </si>
 </sst>
 </file>
@@ -768,10 +780,10 @@
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A2:I51"/>
+  <dimension ref="A2:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="55" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="55" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,7 +792,7 @@
     <col min="2" max="2" width="22.5546875" customWidth="1"/>
     <col min="3" max="3" width="50.44140625" customWidth="1"/>
     <col min="4" max="4" width="3.5546875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="50.44140625" customWidth="1"/>
     <col min="7" max="7" width="3.109375" style="6" customWidth="1"/>
     <col min="8" max="8" width="17.88671875" customWidth="1"/>
@@ -852,21 +864,21 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
@@ -888,7 +900,7 @@
         <v>18</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
@@ -914,7 +926,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="2"/>
@@ -1009,21 +1021,21 @@
         <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="2" t="s">
         <v>33</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="2" t="s">
         <v>33</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
@@ -1038,7 +1050,7 @@
         <v>30</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="2" t="s">
@@ -1049,138 +1061,114 @@
       </c>
     </row>
     <row r="17" spans="2:9" ht="33.6" x14ac:dyDescent="0.4">
-      <c r="B17" t="s">
-        <v>72</v>
+      <c r="B17" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>19</v>
+        <v>48</v>
       </c>
       <c r="D17" s="4"/>
       <c r="E17" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I17" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I17" s="2" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="18" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B18" t="s">
-        <v>66</v>
+      <c r="B18" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="D18" s="4"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="4"/>
       <c r="H18" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B19" t="s">
-        <v>65</v>
+      <c r="B19" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="D19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C20" t="s">
-        <v>69</v>
+      <c r="B20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="D20" s="4"/>
       <c r="G20" s="4"/>
     </row>
     <row r="21" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" t="s">
-        <v>69</v>
+      <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="D21" s="4"/>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
       <c r="B22" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="D22" s="4"/>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
       <c r="B23" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D23" s="4"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B24" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>37</v>
-      </c>
       <c r="D24" s="4"/>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="D25" s="4"/>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B26" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>47</v>
-      </c>
       <c r="D26" s="4"/>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="D27" s="4"/>
       <c r="G27" s="4"/>
     </row>
@@ -1192,12 +1180,12 @@
     </row>
     <row r="29" spans="2:9" ht="19.2" x14ac:dyDescent="0.45">
       <c r="B29" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="4"/>
       <c r="E29" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="4"/>
@@ -1221,43 +1209,76 @@
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="D31" s="4"/>
+      <c r="E31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="B32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>47</v>
+      </c>
       <c r="D32" s="4"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="E32" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="C33" s="2"/>
       <c r="D33" s="4"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="E33" t="s">
+        <v>65</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="E34" t="s">
+        <v>64</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
       <c r="D35" s="4"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="E35" t="s">
+        <v>67</v>
+      </c>
+      <c r="F35" t="s">
+        <v>68</v>
+      </c>
       <c r="G35" s="4"/>
     </row>
     <row r="36" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="E36" t="s">
+        <v>66</v>
+      </c>
+      <c r="F36" t="s">
+        <v>68</v>
+      </c>
       <c r="G36" s="4"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
@@ -1266,8 +1287,12 @@
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G37" s="4"/>
     </row>
     <row r="38" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
@@ -1278,157 +1303,149 @@
       <c r="F38" s="2"/>
       <c r="G38" s="4"/>
     </row>
-    <row r="39" spans="2:9" ht="19.2" x14ac:dyDescent="0.45">
-      <c r="B39" s="8" t="s">
+    <row r="40" spans="2:9" ht="19.2" x14ac:dyDescent="0.45">
+      <c r="B40" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="8" t="s">
+      <c r="C40" s="8"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F39" s="8"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="8" t="s">
+      <c r="F40" s="8"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="I39" s="8"/>
-    </row>
-    <row r="40" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B40" s="3" t="s">
+      <c r="I40" s="8"/>
+    </row>
+    <row r="41" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="B41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D40" s="4"/>
-      <c r="E40" s="3" t="s">
+      <c r="D41" s="4"/>
+      <c r="E41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F41" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G40" s="4"/>
-      <c r="H40" s="3" t="s">
+      <c r="G41" s="4"/>
+      <c r="H41" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I40" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B41" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="4"/>
-      <c r="E41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G41" s="4"/>
-      <c r="H41" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="42" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
       <c r="B42" s="2" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="D42" s="4"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
+      <c r="E42" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="G42" s="4"/>
       <c r="H42" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
       <c r="B43" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D43" s="4"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
       <c r="G43" s="4"/>
       <c r="H43" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="44" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="B44" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D44" s="4"/>
       <c r="G44" s="4"/>
-    </row>
-    <row r="45" spans="2:9" ht="19.2" x14ac:dyDescent="0.45">
-      <c r="H45" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="I45" s="8"/>
-    </row>
-    <row r="46" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="H46" s="3" t="s">
+      <c r="H44" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="D45" s="4"/>
+      <c r="G45" s="4"/>
+    </row>
+    <row r="46" spans="2:9" ht="19.2" x14ac:dyDescent="0.45">
+      <c r="H46" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="I46" s="8"/>
+    </row>
+    <row r="47" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="H47" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I46" s="2" t="s">
+      <c r="I47" s="2" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="H47" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="I47" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="48" spans="2:9" ht="16.8" x14ac:dyDescent="0.4">
       <c r="H48" s="2" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="8:9" ht="16.8" x14ac:dyDescent="0.4">
       <c r="H49" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="8:9" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="H50" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="8:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-    </row>
-    <row r="51" spans="8:9" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
+      <c r="I50" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="B40:C40"/>
     <mergeCell ref="H13:I13"/>
-    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="H46:I46"/>
     <mergeCell ref="B29:C29"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="B2:C2"/>

</xml_diff>